<commit_message>
add notes on Excel templates, sorting,filtering, and subtotals.
</commit_message>
<xml_diff>
--- a/learning-excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
+++ b/learning-excel/Excel Working From Beginner to Advanced - MyFirstExcelWorkbook-01.xlsx
@@ -8,16 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-analysis-foundations\learning-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BE3CCC-10B4-42D1-B2A3-A3DF62E5DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EBF606-9660-47CF-9E4F-C774F63210AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{4EC8B933-5C16-44B8-8BD1-3B03B4E7E629}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{4EC8B933-5C16-44B8-8BD1-3B03B4E7E629}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart Monthly Budget" sheetId="14" r:id="rId1"/>
-    <sheet name="Monthly Budget " sheetId="12" r:id="rId2"/>
-    <sheet name="Copy Exercise" sheetId="3" r:id="rId3"/>
+    <sheet name="Credit card log" sheetId="17" r:id="rId1"/>
+    <sheet name="Chart Monthly Budget" sheetId="14" r:id="rId2"/>
+    <sheet name="Monthly Budget " sheetId="12" r:id="rId3"/>
     <sheet name="Monthly Budget - Print Setting" sheetId="15" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="ColumnTitle1">Data[[#Headers],[Date]]</definedName>
+    <definedName name="LastCol">MATCH(REPT("z",255),#REF!)</definedName>
+    <definedName name="LastRow">MATCH(9.99E+307,#REF!)</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Credit card log'!$3:$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,10 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
-  <si>
-    <t>Montlhy Budget</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Bills</t>
   </si>
@@ -85,18 +88,79 @@
   <si>
     <t>Monthly Budget</t>
   </si>
+  <si>
+    <t>*(does not include interest)</t>
+  </si>
+  <si>
+    <t>Balance*</t>
+  </si>
+  <si>
+    <t>Transaction fees</t>
+  </si>
+  <si>
+    <t>Merchant name</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Enter payments as negative amounts in table, below.</t>
+  </si>
+  <si>
+    <t>Credit Card Name</t>
+  </si>
+  <si>
+    <t>Devreden Bakiye</t>
+  </si>
+  <si>
+    <t>Akbank</t>
+  </si>
+  <si>
+    <t>Market + fatura</t>
+  </si>
+  <si>
+    <t>Çeşitli</t>
+  </si>
+  <si>
+    <t>Alışveriş</t>
+  </si>
+  <si>
+    <t>Yeme-İçme + günlük</t>
+  </si>
+  <si>
+    <t>Diğer</t>
+  </si>
+  <si>
+    <t>İşsizlik maaşı ile ödeme</t>
+  </si>
+  <si>
+    <t>Kardeş maaşı ile ödeme</t>
+  </si>
+  <si>
+    <t>Emekli ile ödeme</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_-&quot;₺&quot;* #,##0_-;\-&quot;₺&quot;* #,##0_-;_-&quot;₺&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;₺&quot;* #,##0.00_-;\-&quot;₺&quot;* #,##0.00_-;_-&quot;₺&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="[$₺-41F]#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +202,114 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +334,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -191,17 +385,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="6" fillId="6" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="6" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -215,14 +493,267 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="17" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="18" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="17" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="17" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="22" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="23" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="24">
+    <cellStyle name="Amount" xfId="11" xr:uid="{067CDA47-A9D5-42FB-8A34-63C555C1FADF}"/>
     <cellStyle name="AwesomeStyle" xfId="3" xr:uid="{65150C0F-7736-4FBF-89DC-FF58D6DB8DAA}"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Currency [0] 2" xfId="19" xr:uid="{5D0D245E-2F0D-4E21-8C61-3992C518CE96}"/>
+    <cellStyle name="Currency 2" xfId="18" xr:uid="{926980A8-E041-4CB0-894A-29AB88A2BD9E}"/>
+    <cellStyle name="Date" xfId="8" xr:uid="{25F744EB-DC48-4D89-AFC7-801DD2C78B12}"/>
+    <cellStyle name="Date 2" xfId="20" xr:uid="{38E01BA8-2E42-474B-9AAA-8A3DC09FFD01}"/>
+    <cellStyle name="Explanatory Text 2" xfId="12" xr:uid="{36721F1D-A737-4058-85A5-1A04265658BF}"/>
+    <cellStyle name="Heading 1 2" xfId="22" xr:uid="{ACF47221-4F9F-43DB-8504-050D7F08E350}"/>
+    <cellStyle name="Heading 2 2" xfId="15" xr:uid="{81E962D4-319E-42CF-9B0E-E90F78347BB1}"/>
+    <cellStyle name="Heading 2 3" xfId="21" xr:uid="{D1913F80-4B17-4F15-8B2D-E41287E263A1}"/>
+    <cellStyle name="Heading 3 2" xfId="10" xr:uid="{2D1BF034-0522-4466-9946-0BE44C63059E}"/>
+    <cellStyle name="Heading 4 Right aligned" xfId="16" xr:uid="{2CE340C6-44BE-4140-B10F-897F4DA2BB0A}"/>
+    <cellStyle name="Loan Summary" xfId="13" xr:uid="{0180723F-9657-4B16-B29F-4C066C3E8BF7}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="6" xr:uid="{C1330DF8-C5F4-46C7-BAFE-F5711B60157F}"/>
+    <cellStyle name="Normal 3" xfId="17" xr:uid="{7586D2E5-82AE-430B-BA29-EF0914C24989}"/>
+    <cellStyle name="Number" xfId="9" xr:uid="{7E2D30BE-C2D2-4D7A-8DD3-ADB26E3534FA}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="14" xr:uid="{8B497EA1-7954-47E8-990D-E6A99301CE83}"/>
+    <cellStyle name="Table Amount" xfId="7" xr:uid="{79E33E4A-2F9C-4099-A328-91B9FD2F580E}"/>
+    <cellStyle name="Title 2" xfId="23" xr:uid="{FE0C7761-2F05-42B5-8B23-D4DD8A581DE8}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -243,8 +774,273 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="[$₺-41F]#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="[$₺-41F]#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="238"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="mediumDashed">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+        <horizontal style="medium">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.24994659260841701"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.24994659260841701"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Loan Amortization Schedule" pivot="0" count="3" xr9:uid="{68D86AE2-33E2-466F-A3D3-12AE868A916E}">
+      <tableStyleElement type="wholeTable" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="totalRow" dxfId="23"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1" pivot="0" count="6" xr9:uid="{A2562EC2-7814-4264-B617-2D493C35B01F}">
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="lastColumn" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="lastTotalCell" dxfId="17"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8977,8 +9773,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="344634" y="0"/>
-          <a:ext cx="3905862" cy="2743200"/>
+          <a:off x="342899" y="0"/>
+          <a:ext cx="3886200" cy="2743200"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -9056,8 +9852,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="155713" y="822960"/>
-          <a:ext cx="1378539" cy="1097280"/>
+          <a:off x="154930" y="822960"/>
+          <a:ext cx="1371600" cy="1097280"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9191,8 +9987,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="209278" y="876525"/>
-        <a:ext cx="1271409" cy="990150"/>
+        <a:off x="208495" y="876525"/>
+        <a:ext cx="1264470" cy="990150"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4AF387EC-071A-495C-B3C8-8FD928F3F851}">
@@ -9202,8 +9998,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1608296" y="822960"/>
-          <a:ext cx="1378539" cy="1097280"/>
+          <a:off x="1600199" y="822960"/>
+          <a:ext cx="1371600" cy="1097280"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9337,8 +10133,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1661861" y="876525"/>
-        <a:ext cx="1271409" cy="990150"/>
+        <a:off x="1653764" y="876525"/>
+        <a:ext cx="1264470" cy="990150"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{DE0BD434-849F-4135-AAA4-AFA4E216BFC6}">
@@ -9348,8 +10144,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3060878" y="822960"/>
-          <a:ext cx="1378539" cy="1097280"/>
+          <a:off x="3045469" y="822960"/>
+          <a:ext cx="1371600" cy="1097280"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9483,8 +10279,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3114443" y="876525"/>
-        <a:ext cx="1271409" cy="990150"/>
+        <a:off x="3099034" y="876525"/>
+        <a:ext cx="1264470" cy="990150"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -9506,8 +10302,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="515036" y="0"/>
-          <a:ext cx="5837082" cy="4009531"/>
+          <a:off x="557184" y="0"/>
+          <a:ext cx="6314761" cy="3987017"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -9585,8 +10381,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3950" y="1202859"/>
-          <a:ext cx="2203932" cy="1603812"/>
+          <a:off x="1587" y="1196105"/>
+          <a:ext cx="2379190" cy="1594806"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9657,12 +10453,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="83820" tIns="83820" rIns="83820" bIns="83820" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="87630" tIns="87630" rIns="87630" bIns="87630" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="977900">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1022350">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9675,13 +10471,13 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="2200" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="2300" kern="1200"/>
             <a:t>Collect Income</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="2200" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2300" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9694,13 +10490,13 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Salary/ side income</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9713,15 +10509,15 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Set a target amount</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="82242" y="1281151"/>
-        <a:ext cx="2047348" cy="1447228"/>
+        <a:off x="79439" y="1273957"/>
+        <a:ext cx="2223486" cy="1439102"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4AF387EC-071A-495C-B3C8-8FD928F3F851}">
@@ -9731,8 +10527,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2331611" y="1202859"/>
-          <a:ext cx="2203932" cy="1603812"/>
+          <a:off x="2524970" y="1196105"/>
+          <a:ext cx="2379190" cy="1594806"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9803,12 +10599,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="83820" tIns="83820" rIns="83820" bIns="83820" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="87630" tIns="87630" rIns="87630" bIns="87630" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="977900">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1022350">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9821,13 +10617,13 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="2200" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="2300" kern="1200"/>
             <a:t>Plan Spending</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="2200" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2300" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9840,13 +10636,13 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Bills</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9859,15 +10655,15 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Daily needs</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2409903" y="1281151"/>
-        <a:ext cx="2047348" cy="1447228"/>
+        <a:off x="2602822" y="1273957"/>
+        <a:ext cx="2223486" cy="1439102"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{DE0BD434-849F-4135-AAA4-AFA4E216BFC6}">
@@ -9877,8 +10673,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4659273" y="1202859"/>
-          <a:ext cx="2203932" cy="1603812"/>
+          <a:off x="5048353" y="1196105"/>
+          <a:ext cx="2379190" cy="1594806"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9949,12 +10745,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="83820" tIns="83820" rIns="83820" bIns="83820" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="87630" tIns="87630" rIns="87630" bIns="87630" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="977900">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1022350">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9967,13 +10763,13 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="2200" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="2300" kern="1200"/>
             <a:t>Review &amp; Adjust</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="2200" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2300" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -9986,13 +10782,13 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Money left</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="755650">
+          <a:pPr marL="171450" lvl="1" indent="-171450" algn="l" defTabSz="800100">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -10005,15 +10801,15 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1700" kern="1200"/>
+            <a:rPr lang="tr-TR" sz="1800" kern="1200"/>
             <a:t>Cut unnecessary spending</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4737565" y="1281151"/>
-        <a:ext cx="2047348" cy="1447228"/>
+        <a:off x="5126205" y="1273957"/>
+        <a:ext cx="2223486" cy="1439102"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -12564,9 +13360,308 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>728383</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1266263</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F77386F6-359E-41AF-8D81-D324E0F595D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2233333" y="0"/>
+          <a:ext cx="3033430" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="3600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Credit Card Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>227610</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7733</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="10517860" cy="1141104"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Group 2" descr="decorative element with hand holding credit card">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C06B87-7A68-485E-BAAD-81FFB7B5F7EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="227610" y="7733"/>
+          <a:ext cx="10517860" cy="1141104"/>
+          <a:chOff x="227610" y="7733"/>
+          <a:chExt cx="10484748" cy="1139743"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Group 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D14587C6-797C-65E4-ECDC-3953710078B3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="227919" y="7733"/>
+            <a:ext cx="10484439" cy="1137269"/>
+            <a:chOff x="224117" y="0"/>
+            <a:chExt cx="10467089" cy="1135268"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Rectangle 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E17A6D2E-70CA-86D9-ECEC-F3AC7E0ACF40}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="224117" y="14655"/>
+              <a:ext cx="10467089" cy="1120613"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="tx2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D864E98-5C5E-A6F8-75DB-FE901E91FC7A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1826071" y="0"/>
+              <a:ext cx="8651051" cy="1120588"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="4400">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                </a:rPr>
+                <a:t>Woodgrove</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="4400">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                </a:rPr>
+                <a:t> Bank</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="4400">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                </a:rPr>
+                <a:t> debit card</a:t>
+              </a:r>
+              <a:endParaRPr lang="pl-PL" sz="4400">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Picture 4" descr="hand holding credit card">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{718BAD77-46BF-01AF-D5A1-5822A41CD539}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="227610" y="159357"/>
+            <a:ext cx="1398191" cy="988119"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9296400" cy="6071251"/>
+    <xdr:ext cx="9297051" cy="6073205"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -12595,7 +13690,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -12821,7 +13916,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -13045,6 +14140,37 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB789D22-759C-4849-A1E2-9F97DB7CAD27}" name="Data" displayName="Data" ref="B3:G12" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14" headerRowCellStyle="Normal" dataCellStyle="Normal" totalsRowCellStyle="Normal">
+  <autoFilter ref="B3:G11" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="5" dataCellStyle="Date">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="12" totalsRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Amount" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Merchant name" dataDxfId="11" totalsRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Transaction fees" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Balance*" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency [0]">
+      <calculatedColumnFormula>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Enter credit card payment details such as Date, Description, Amount, Merchant Name, and Transaction fees in this table. Balance excluding interest is automatically calculated"/>
+    </ext>
+  </extLst>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13413,6 +14539,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD56CCD-EE54-4BDE-8496-779611148FD7}">
+  <sheetPr>
+    <tabColor theme="4"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:G13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="11.28515625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <v>46023</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="25">
+        <v>40000</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
+        <v>46024</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="25">
+        <v>8000</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>46032</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="25">
+        <v>12000</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
+        <v>46043</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="25">
+        <v>14000</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>74000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
+        <v>46051</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="25">
+        <v>6000</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
+        <v>46028</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="25">
+        <v>-18230</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>61770</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>46040</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="26">
+        <v>-25000</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>36770</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>46048</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="26">
+        <v>-25000</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <f>IFERROR(IF(ROW()-ROW(Data[[#Headers],[Balance*]])=1,Data[[#This Row],[Transaction fees]]+Data[[#This Row],[Amount]],SUM(INDEX(Data[Amount],1,1):Data[[#This Row],[Amount]],INDEX(Data[Transaction fees],1,1):Data[[#This Row],[Transaction fees]])), "")</f>
+        <v>11770</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23">
+        <f>SUBTOTAL(109,Data[Amount])</f>
+        <v>11770</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23">
+        <f>SUBTOTAL(109,Data[Transaction fees])</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="12"/>
+      <c r="G13" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Balance excluding interest is automatically calculated in this column under this heading" sqref="G3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Transaction fees in this column under this heading" sqref="F3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Merchant name in this column under this heading" sqref="E3" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Amount in this column under this heading" sqref="D3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter Credit Card Name to update the title" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a credit card log in this worksheet" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>
+  <pageSetup scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="B4:B6" calculatedColumn="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD3905B-E95B-4636-863D-328414AE3C59}">
   <dimension ref="B3:G17"/>
   <sheetViews>
@@ -13432,196 +14835,196 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="37.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
         <v>45292</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>45323</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>45717</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
         <v>48000</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>25000</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>35000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f t="shared" ref="F6:F12" si="0">SUM(C6:E6)</f>
         <v>108000</v>
       </c>
-      <c r="G6" s="6">
-        <f>F6/$F$12</f>
+      <c r="G6" s="4">
+        <f t="shared" ref="G6:G12" si="1">F6/$F$12</f>
         <v>0.52735919997656178</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
         <v>1000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>950</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>950</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>2900</v>
       </c>
-      <c r="G7" s="6">
-        <f>F7/$F$12</f>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
         <v>1.4160571110481752E-2</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
         <v>350</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>4324</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>120</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>4794</v>
       </c>
-      <c r="G8" s="6">
-        <f>F8/$F$12</f>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
         <v>2.340888893229294E-2</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
         <v>1500</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>1500</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>1400</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>4400</v>
       </c>
-      <c r="G9" s="6">
-        <f>F9/$F$12</f>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
         <v>2.1485004443489556E-2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
         <v>22000</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>22000</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>24000</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>68000</v>
       </c>
-      <c r="G10" s="6">
-        <f>F10/$F$12</f>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
         <v>0.33204097776302038</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
         <v>5500</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>5850</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>5350</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>16700</v>
       </c>
-      <c r="G11" s="6">
-        <f>F11/$F$12</f>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
         <v>8.1545357774153546E-2</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
         <f>SUM(C6:C11)</f>
         <v>78350</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" ref="D12:E12" si="1">SUM(D6:D11)</f>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:E12" si="2">SUM(D6:D11)</f>
         <v>59624</v>
       </c>
-      <c r="E12" s="4">
-        <f t="shared" si="1"/>
+      <c r="E12" s="2">
+        <f t="shared" si="2"/>
         <v>66820</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>204794</v>
       </c>
-      <c r="G12" s="6">
-        <f>F12/$F$12</f>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>9</v>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C14">
         <f>MIN(C6:C11)</f>
@@ -13639,11 +15042,11 @@
         <f>MIN(F6:F11)</f>
         <v>2900</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>10</v>
+      <c r="B15" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C15">
         <f>MAX(C6:C11)</f>
@@ -13663,8 +15066,8 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>11</v>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C16">
         <f>AVERAGE(C6:C11)</f>
@@ -13684,8 +15087,8 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>12</v>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C17">
         <f>COUNT(C6:C11)</f>
@@ -13709,7 +15112,7 @@
     <mergeCell ref="B3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:E11">
-    <cfRule type="aboveAverage" dxfId="1" priority="1"/>
+    <cfRule type="aboveAverage" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
@@ -13720,294 +15123,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63FC743-2487-47E6-ADBA-53D754771889}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45292</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45323</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45717</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>48000</v>
-      </c>
-      <c r="C4">
-        <v>25000</v>
-      </c>
-      <c r="D4">
-        <v>35000</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E10" si="0">SUM(B4:D4)</f>
-        <v>108000</v>
-      </c>
-      <c r="F4" s="3" t="e">
-        <f t="shared" ref="F4:F10" si="1">E4/$F$12</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>950</v>
-      </c>
-      <c r="D5">
-        <v>950</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>2900</v>
-      </c>
-      <c r="F5" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>350</v>
-      </c>
-      <c r="C6">
-        <v>4324</v>
-      </c>
-      <c r="D6">
-        <v>120</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>4794</v>
-      </c>
-      <c r="F6" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1500</v>
-      </c>
-      <c r="C7">
-        <v>1500</v>
-      </c>
-      <c r="D7">
-        <v>1400</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>4400</v>
-      </c>
-      <c r="F7" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>22000</v>
-      </c>
-      <c r="C8">
-        <v>22000</v>
-      </c>
-      <c r="D8">
-        <v>24000</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>68000</v>
-      </c>
-      <c r="F8" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>5500</v>
-      </c>
-      <c r="C9">
-        <v>5850</v>
-      </c>
-      <c r="D9">
-        <v>5350</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>16700</v>
-      </c>
-      <c r="F9" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <f>SUM(B4:B9)</f>
-        <v>78350</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:D10" si="2">SUM(C4:C9)</f>
-        <v>59624</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>66820</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>204794</v>
-      </c>
-      <c r="F10" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <f>MIN(B4:B9)</f>
-        <v>350</v>
-      </c>
-      <c r="C12">
-        <f>MIN(C4:C9)</f>
-        <v>950</v>
-      </c>
-      <c r="D12">
-        <f>MIN(D4:D9)</f>
-        <v>120</v>
-      </c>
-      <c r="E12">
-        <f>MIN(E4:E9)</f>
-        <v>2900</v>
-      </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <f>MAX(B4:B9)</f>
-        <v>48000</v>
-      </c>
-      <c r="C13">
-        <f>MAX(C4:C9)</f>
-        <v>25000</v>
-      </c>
-      <c r="D13">
-        <f>MAX(D4:D9)</f>
-        <v>35000</v>
-      </c>
-      <c r="E13">
-        <f>MAX(E4:E9)</f>
-        <v>108000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <f>AVERAGE(B4:B9)</f>
-        <v>13058.333333333334</v>
-      </c>
-      <c r="C14">
-        <f>AVERAGE(C4:C9)</f>
-        <v>9937.3333333333339</v>
-      </c>
-      <c r="D14">
-        <f>AVERAGE(D4:D9)</f>
-        <v>11136.666666666666</v>
-      </c>
-      <c r="E14">
-        <f>AVERAGE(E4:E9)</f>
-        <v>34132.333333333336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <f>COUNT(B4:B9)</f>
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <f>COUNT(C4:C9)</f>
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <f>COUNT(D4:D9)</f>
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <f>COUNT(E4:E9)</f>
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAF6158-2E65-4CED-8DF1-A23D38422DE5}">
   <dimension ref="B18:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14025,196 +15146,196 @@
   </cols>
   <sheetData>
     <row r="18" spans="2:7" ht="37.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9">
+      <c r="B20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
         <v>45292</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>45323</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>45717</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
         <v>48000</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>25000</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>35000</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="2">
         <f t="shared" ref="F21:F27" si="0">SUM(C21:E21)</f>
         <v>108000</v>
       </c>
-      <c r="G21" s="6">
-        <f>F21/$F$27</f>
+      <c r="G21" s="4">
+        <f t="shared" ref="G21:G27" si="1">F21/$F$27</f>
         <v>0.52735919997656178</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
         <v>1000</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="3">
         <v>950</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="3">
         <v>950</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>2900</v>
       </c>
-      <c r="G22" s="6">
-        <f>F22/$F$27</f>
+      <c r="G22" s="4">
+        <f t="shared" si="1"/>
         <v>1.4160571110481752E-2</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="5">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3">
         <v>350</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="3">
         <v>4324</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="3">
         <v>120</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>4794</v>
       </c>
-      <c r="G23" s="6">
-        <f>F23/$F$27</f>
+      <c r="G23" s="4">
+        <f t="shared" si="1"/>
         <v>2.340888893229294E-2</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
         <v>1500</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <v>1500</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="3">
         <v>1400</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>4400</v>
       </c>
-      <c r="G24" s="6">
-        <f>F24/$F$27</f>
+      <c r="G24" s="4">
+        <f t="shared" si="1"/>
         <v>2.1485004443489556E-2</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
         <v>22000</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="3">
         <v>22000</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="3">
         <v>24000</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>68000</v>
       </c>
-      <c r="G25" s="6">
-        <f>F25/$F$27</f>
+      <c r="G25" s="4">
+        <f t="shared" si="1"/>
         <v>0.33204097776302038</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3">
         <v>5500</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="3">
         <v>5850</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="3">
         <v>5350</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>16700</v>
       </c>
-      <c r="G26" s="6">
-        <f>F26/$F$27</f>
+      <c r="G26" s="4">
+        <f t="shared" si="1"/>
         <v>8.1545357774153546E-2</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="4">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2">
         <f>SUM(C21:C26)</f>
         <v>78350</v>
       </c>
-      <c r="D27" s="4">
-        <f t="shared" ref="D27:E27" si="1">SUM(D21:D26)</f>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:E27" si="2">SUM(D21:D26)</f>
         <v>59624</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" si="1"/>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
         <v>66820</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="2">
         <f t="shared" si="0"/>
         <v>204794</v>
       </c>
-      <c r="G27" s="6">
-        <f>F27/$F$27</f>
+      <c r="G27" s="4">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>9</v>
+      <c r="B29" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C29">
         <f>MIN(C21:C26)</f>
@@ -14232,11 +15353,11 @@
         <f>MIN(F21:F26)</f>
         <v>2900</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>10</v>
+      <c r="B30" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C30">
         <f>MAX(C21:C26)</f>
@@ -14256,8 +15377,8 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
-        <v>11</v>
+      <c r="B31" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C31">
         <f>AVERAGE(C21:C26)</f>
@@ -14277,8 +15398,8 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
-        <v>12</v>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C32">
         <f>COUNT(C21:C26)</f>
@@ -14302,7 +15423,7 @@
     <mergeCell ref="B18:G18"/>
   </mergeCells>
   <conditionalFormatting sqref="C21:E26">
-    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+    <cfRule type="aboveAverage" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>